<commit_message>
On branch main  Your branch is up to date with 'origin/main'.  Changes to be committed: 	deleted:    "\345\256\236\346\210\2301/BOOM\345\255\246\344\271\240.zip"
</commit_message>
<xml_diff>
--- a/实战1/真题模拟/2023国赛C/解题代码/单品销量统计.xlsx
+++ b/实战1/真题模拟/2023国赛C/解题代码/单品销量统计.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E247"/>
+  <dimension ref="A1:D247"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,11 +454,6 @@
           <t>单品日最大销量</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Cluster</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -475,9 +470,6 @@
       <c r="D2" t="n">
         <v>16.1</v>
       </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -494,9 +486,6 @@
       <c r="D3" t="n">
         <v>5.8</v>
       </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -513,9 +502,6 @@
       <c r="D4" t="n">
         <v>4</v>
       </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -532,9 +518,6 @@
       <c r="D5" t="n">
         <v>43.6</v>
       </c>
-      <c r="E5" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -551,9 +534,6 @@
       <c r="D6" t="n">
         <v>118</v>
       </c>
-      <c r="E6" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -570,9 +550,6 @@
       <c r="D7" t="n">
         <v>15.1</v>
       </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -589,9 +566,6 @@
       <c r="D8" t="n">
         <v>3</v>
       </c>
-      <c r="E8" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -608,9 +582,6 @@
       <c r="D9" t="n">
         <v>76.59999999999999</v>
       </c>
-      <c r="E9" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -627,9 +598,6 @@
       <c r="D10" t="n">
         <v>166</v>
       </c>
-      <c r="E10" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -646,9 +614,6 @@
       <c r="D11" t="n">
         <v>76.40000000000001</v>
       </c>
-      <c r="E11" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -665,9 +630,6 @@
       <c r="D12" t="n">
         <v>151</v>
       </c>
-      <c r="E12" t="n">
-        <v>2</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -684,9 +646,6 @@
       <c r="D13" t="n">
         <v>4.6</v>
       </c>
-      <c r="E13" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -703,9 +662,6 @@
       <c r="D14" t="n">
         <v>138.5</v>
       </c>
-      <c r="E14" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -722,9 +678,6 @@
       <c r="D15" t="n">
         <v>4.1</v>
       </c>
-      <c r="E15" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -741,9 +694,6 @@
       <c r="D16" t="n">
         <v>2</v>
       </c>
-      <c r="E16" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -760,9 +710,6 @@
       <c r="D17" t="n">
         <v>157.1</v>
       </c>
-      <c r="E17" t="n">
-        <v>2</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -779,9 +726,6 @@
       <c r="D18" t="n">
         <v>25.2</v>
       </c>
-      <c r="E18" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -798,9 +742,6 @@
       <c r="D19" t="n">
         <v>13.9</v>
       </c>
-      <c r="E19" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -817,9 +758,6 @@
       <c r="D20" t="n">
         <v>6.2</v>
       </c>
-      <c r="E20" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -836,9 +774,6 @@
       <c r="D21" t="n">
         <v>7.3</v>
       </c>
-      <c r="E21" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -855,9 +790,6 @@
       <c r="D22" t="n">
         <v>6</v>
       </c>
-      <c r="E22" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -874,9 +806,6 @@
       <c r="D23" t="n">
         <v>57</v>
       </c>
-      <c r="E23" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -893,9 +822,6 @@
       <c r="D24" t="n">
         <v>2.2</v>
       </c>
-      <c r="E24" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -912,9 +838,6 @@
       <c r="D25" t="n">
         <v>10</v>
       </c>
-      <c r="E25" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -931,9 +854,6 @@
       <c r="D26" t="n">
         <v>12.8</v>
       </c>
-      <c r="E26" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -950,9 +870,6 @@
       <c r="D27" t="n">
         <v>4.3</v>
       </c>
-      <c r="E27" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -969,9 +886,6 @@
       <c r="D28" t="n">
         <v>18.8</v>
       </c>
-      <c r="E28" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -988,9 +902,6 @@
       <c r="D29" t="n">
         <v>11</v>
       </c>
-      <c r="E29" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1007,9 +918,6 @@
       <c r="D30" t="n">
         <v>15</v>
       </c>
-      <c r="E30" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1026,9 +934,6 @@
       <c r="D31" t="n">
         <v>244.4</v>
       </c>
-      <c r="E31" t="n">
-        <v>2</v>
-      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1045,9 +950,6 @@
       <c r="D32" t="n">
         <v>7.2</v>
       </c>
-      <c r="E32" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1064,9 +966,6 @@
       <c r="D33" t="n">
         <v>4.9</v>
       </c>
-      <c r="E33" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1083,9 +982,6 @@
       <c r="D34" t="n">
         <v>34.3</v>
       </c>
-      <c r="E34" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1102,9 +998,6 @@
       <c r="D35" t="n">
         <v>36</v>
       </c>
-      <c r="E35" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1121,9 +1014,6 @@
       <c r="D36" t="n">
         <v>153</v>
       </c>
-      <c r="E36" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1140,9 +1030,6 @@
       <c r="D37" t="n">
         <v>5.1</v>
       </c>
-      <c r="E37" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1159,9 +1046,6 @@
       <c r="D38" t="n">
         <v>25</v>
       </c>
-      <c r="E38" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1178,9 +1062,6 @@
       <c r="D39" t="n">
         <v>4.2</v>
       </c>
-      <c r="E39" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1197,9 +1078,6 @@
       <c r="D40" t="n">
         <v>1.3</v>
       </c>
-      <c r="E40" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1216,9 +1094,6 @@
       <c r="D41" t="n">
         <v>21</v>
       </c>
-      <c r="E41" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1235,9 +1110,6 @@
       <c r="D42" t="n">
         <v>15</v>
       </c>
-      <c r="E42" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1254,9 +1126,6 @@
       <c r="D43" t="n">
         <v>407</v>
       </c>
-      <c r="E43" t="n">
-        <v>2</v>
-      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1273,9 +1142,6 @@
       <c r="D44" t="n">
         <v>11.5</v>
       </c>
-      <c r="E44" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1292,9 +1158,6 @@
       <c r="D45" t="n">
         <v>15</v>
       </c>
-      <c r="E45" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1311,9 +1174,6 @@
       <c r="D46" t="n">
         <v>7.6</v>
       </c>
-      <c r="E46" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1330,9 +1190,6 @@
       <c r="D47" t="n">
         <v>56</v>
       </c>
-      <c r="E47" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1349,9 +1206,6 @@
       <c r="D48" t="n">
         <v>30.5</v>
       </c>
-      <c r="E48" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1368,9 +1222,6 @@
       <c r="D49" t="n">
         <v>210</v>
       </c>
-      <c r="E49" t="n">
-        <v>2</v>
-      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1387,9 +1238,6 @@
       <c r="D50" t="n">
         <v>24.3</v>
       </c>
-      <c r="E50" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1406,9 +1254,6 @@
       <c r="D51" t="n">
         <v>15</v>
       </c>
-      <c r="E51" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1425,9 +1270,6 @@
       <c r="D52" t="n">
         <v>70</v>
       </c>
-      <c r="E52" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1444,9 +1286,6 @@
       <c r="D53" t="n">
         <v>45</v>
       </c>
-      <c r="E53" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1463,9 +1302,6 @@
       <c r="D54" t="n">
         <v>10.3</v>
       </c>
-      <c r="E54" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1482,9 +1318,6 @@
       <c r="D55" t="n">
         <v>4</v>
       </c>
-      <c r="E55" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1501,9 +1334,6 @@
       <c r="D56" t="n">
         <v>16.8</v>
       </c>
-      <c r="E56" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1520,9 +1350,6 @@
       <c r="D57" t="n">
         <v>2</v>
       </c>
-      <c r="E57" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1539,9 +1366,6 @@
       <c r="D58" t="n">
         <v>27.9</v>
       </c>
-      <c r="E58" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1558,9 +1382,6 @@
       <c r="D59" t="n">
         <v>12.9</v>
       </c>
-      <c r="E59" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1577,9 +1398,6 @@
       <c r="D60" t="n">
         <v>35.4</v>
       </c>
-      <c r="E60" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1596,9 +1414,6 @@
       <c r="D61" t="n">
         <v>42.4</v>
       </c>
-      <c r="E61" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1615,9 +1430,6 @@
       <c r="D62" t="n">
         <v>17.4</v>
       </c>
-      <c r="E62" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1634,9 +1446,6 @@
       <c r="D63" t="n">
         <v>3</v>
       </c>
-      <c r="E63" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1653,9 +1462,6 @@
       <c r="D64" t="n">
         <v>9</v>
       </c>
-      <c r="E64" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1672,9 +1478,6 @@
       <c r="D65" t="n">
         <v>111</v>
       </c>
-      <c r="E65" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1691,9 +1494,6 @@
       <c r="D66" t="n">
         <v>89.5</v>
       </c>
-      <c r="E66" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1710,9 +1510,6 @@
       <c r="D67" t="n">
         <v>20</v>
       </c>
-      <c r="E67" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1729,9 +1526,6 @@
       <c r="D68" t="n">
         <v>47.6</v>
       </c>
-      <c r="E68" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1748,9 +1542,6 @@
       <c r="D69" t="n">
         <v>1.4</v>
       </c>
-      <c r="E69" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1767,9 +1558,6 @@
       <c r="D70" t="n">
         <v>1.8</v>
       </c>
-      <c r="E70" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -1786,9 +1574,6 @@
       <c r="D71" t="n">
         <v>9</v>
       </c>
-      <c r="E71" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -1805,9 +1590,6 @@
       <c r="D72" t="n">
         <v>0.4</v>
       </c>
-      <c r="E72" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -1824,9 +1606,6 @@
       <c r="D73" t="n">
         <v>4.9</v>
       </c>
-      <c r="E73" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -1843,9 +1622,6 @@
       <c r="D74" t="n">
         <v>144</v>
       </c>
-      <c r="E74" t="n">
-        <v>2</v>
-      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -1862,9 +1638,6 @@
       <c r="D75" t="n">
         <v>10</v>
       </c>
-      <c r="E75" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -1881,9 +1654,6 @@
       <c r="D76" t="n">
         <v>3</v>
       </c>
-      <c r="E76" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -1900,9 +1670,6 @@
       <c r="D77" t="n">
         <v>1</v>
       </c>
-      <c r="E77" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -1919,9 +1686,6 @@
       <c r="D78" t="n">
         <v>131</v>
       </c>
-      <c r="E78" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -1938,9 +1702,6 @@
       <c r="D79" t="n">
         <v>12</v>
       </c>
-      <c r="E79" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -1957,9 +1718,6 @@
       <c r="D80" t="n">
         <v>11.2</v>
       </c>
-      <c r="E80" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -1976,9 +1734,6 @@
       <c r="D81" t="n">
         <v>1</v>
       </c>
-      <c r="E81" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -1995,9 +1750,6 @@
       <c r="D82" t="n">
         <v>4.8</v>
       </c>
-      <c r="E82" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -2014,9 +1766,6 @@
       <c r="D83" t="n">
         <v>3.6</v>
       </c>
-      <c r="E83" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -2033,9 +1782,6 @@
       <c r="D84" t="n">
         <v>37</v>
       </c>
-      <c r="E84" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -2052,9 +1798,6 @@
       <c r="D85" t="n">
         <v>25</v>
       </c>
-      <c r="E85" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -2071,9 +1814,6 @@
       <c r="D86" t="n">
         <v>57</v>
       </c>
-      <c r="E86" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -2090,9 +1830,6 @@
       <c r="D87" t="n">
         <v>40</v>
       </c>
-      <c r="E87" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -2109,9 +1846,6 @@
       <c r="D88" t="n">
         <v>30</v>
       </c>
-      <c r="E88" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -2128,9 +1862,6 @@
       <c r="D89" t="n">
         <v>45</v>
       </c>
-      <c r="E89" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -2147,9 +1878,6 @@
       <c r="D90" t="n">
         <v>5.8</v>
       </c>
-      <c r="E90" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -2166,9 +1894,6 @@
       <c r="D91" t="n">
         <v>3.5</v>
       </c>
-      <c r="E91" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -2185,9 +1910,6 @@
       <c r="D92" t="n">
         <v>3</v>
       </c>
-      <c r="E92" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -2204,9 +1926,6 @@
       <c r="D93" t="n">
         <v>1.6</v>
       </c>
-      <c r="E93" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -2223,9 +1942,6 @@
       <c r="D94" t="n">
         <v>4</v>
       </c>
-      <c r="E94" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -2242,9 +1958,6 @@
       <c r="D95" t="n">
         <v>66</v>
       </c>
-      <c r="E95" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -2261,9 +1974,6 @@
       <c r="D96" t="n">
         <v>27.3</v>
       </c>
-      <c r="E96" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -2280,9 +1990,6 @@
       <c r="D97" t="n">
         <v>2</v>
       </c>
-      <c r="E97" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -2299,9 +2006,6 @@
       <c r="D98" t="n">
         <v>1</v>
       </c>
-      <c r="E98" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -2318,9 +2022,6 @@
       <c r="D99" t="n">
         <v>0.9</v>
       </c>
-      <c r="E99" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -2337,9 +2038,6 @@
       <c r="D100" t="n">
         <v>71.59999999999999</v>
       </c>
-      <c r="E100" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -2356,9 +2054,6 @@
       <c r="D101" t="n">
         <v>1.2</v>
       </c>
-      <c r="E101" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -2375,9 +2070,6 @@
       <c r="D102" t="n">
         <v>5</v>
       </c>
-      <c r="E102" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -2394,9 +2086,6 @@
       <c r="D103" t="n">
         <v>8</v>
       </c>
-      <c r="E103" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -2413,9 +2102,6 @@
       <c r="D104" t="n">
         <v>18</v>
       </c>
-      <c r="E104" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -2432,9 +2118,6 @@
       <c r="D105" t="n">
         <v>48</v>
       </c>
-      <c r="E105" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -2451,9 +2134,6 @@
       <c r="D106" t="n">
         <v>23.2</v>
       </c>
-      <c r="E106" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -2470,9 +2150,6 @@
       <c r="D107" t="n">
         <v>0.3</v>
       </c>
-      <c r="E107" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -2489,9 +2166,6 @@
       <c r="D108" t="n">
         <v>2.5</v>
       </c>
-      <c r="E108" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -2508,9 +2182,6 @@
       <c r="D109" t="n">
         <v>61.5</v>
       </c>
-      <c r="E109" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -2527,9 +2198,6 @@
       <c r="D110" t="n">
         <v>59</v>
       </c>
-      <c r="E110" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -2546,9 +2214,6 @@
       <c r="D111" t="n">
         <v>2.5</v>
       </c>
-      <c r="E111" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -2565,9 +2230,6 @@
       <c r="D112" t="n">
         <v>1.4</v>
       </c>
-      <c r="E112" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -2584,9 +2246,6 @@
       <c r="D113" t="n">
         <v>1.6</v>
       </c>
-      <c r="E113" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -2603,9 +2262,6 @@
       <c r="D114" t="n">
         <v>0.4</v>
       </c>
-      <c r="E114" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -2622,9 +2278,6 @@
       <c r="D115" t="n">
         <v>1.5</v>
       </c>
-      <c r="E115" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -2641,9 +2294,6 @@
       <c r="D116" t="n">
         <v>3</v>
       </c>
-      <c r="E116" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -2660,9 +2310,6 @@
       <c r="D117" t="n">
         <v>51.5</v>
       </c>
-      <c r="E117" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -2679,9 +2326,6 @@
       <c r="D118" t="n">
         <v>109.4</v>
       </c>
-      <c r="E118" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -2698,9 +2342,6 @@
       <c r="D119" t="n">
         <v>2</v>
       </c>
-      <c r="E119" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -2717,9 +2358,6 @@
       <c r="D120" t="n">
         <v>1.5</v>
       </c>
-      <c r="E120" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -2736,9 +2374,6 @@
       <c r="D121" t="n">
         <v>7.8</v>
       </c>
-      <c r="E121" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -2755,9 +2390,6 @@
       <c r="D122" t="n">
         <v>16</v>
       </c>
-      <c r="E122" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -2774,9 +2406,6 @@
       <c r="D123" t="n">
         <v>18.4</v>
       </c>
-      <c r="E123" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -2793,9 +2422,6 @@
       <c r="D124" t="n">
         <v>15</v>
       </c>
-      <c r="E124" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -2812,9 +2438,6 @@
       <c r="D125" t="n">
         <v>113.8</v>
       </c>
-      <c r="E125" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -2831,9 +2454,6 @@
       <c r="D126" t="n">
         <v>12.3</v>
       </c>
-      <c r="E126" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -2850,9 +2470,6 @@
       <c r="D127" t="n">
         <v>10</v>
       </c>
-      <c r="E127" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -2869,9 +2486,6 @@
       <c r="D128" t="n">
         <v>0.4</v>
       </c>
-      <c r="E128" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -2888,9 +2502,6 @@
       <c r="D129" t="n">
         <v>7.2</v>
       </c>
-      <c r="E129" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -2907,9 +2518,6 @@
       <c r="D130" t="n">
         <v>9.5</v>
       </c>
-      <c r="E130" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -2926,9 +2534,6 @@
       <c r="D131" t="n">
         <v>3</v>
       </c>
-      <c r="E131" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -2945,9 +2550,6 @@
       <c r="D132" t="n">
         <v>0.7</v>
       </c>
-      <c r="E132" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -2964,9 +2566,6 @@
       <c r="D133" t="n">
         <v>2.7</v>
       </c>
-      <c r="E133" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -2983,9 +2582,6 @@
       <c r="D134" t="n">
         <v>4.7</v>
       </c>
-      <c r="E134" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -3002,9 +2598,6 @@
       <c r="D135" t="n">
         <v>55.2</v>
       </c>
-      <c r="E135" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -3021,9 +2614,6 @@
       <c r="D136" t="n">
         <v>35</v>
       </c>
-      <c r="E136" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -3040,9 +2630,6 @@
       <c r="D137" t="n">
         <v>31</v>
       </c>
-      <c r="E137" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -3059,9 +2646,6 @@
       <c r="D138" t="n">
         <v>2</v>
       </c>
-      <c r="E138" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -3078,9 +2662,6 @@
       <c r="D139" t="n">
         <v>1</v>
       </c>
-      <c r="E139" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -3097,9 +2678,6 @@
       <c r="D140" t="n">
         <v>1.2</v>
       </c>
-      <c r="E140" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -3116,9 +2694,6 @@
       <c r="D141" t="n">
         <v>4.9</v>
       </c>
-      <c r="E141" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -3135,9 +2710,6 @@
       <c r="D142" t="n">
         <v>250</v>
       </c>
-      <c r="E142" t="n">
-        <v>2</v>
-      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -3154,9 +2726,6 @@
       <c r="D143" t="n">
         <v>9.4</v>
       </c>
-      <c r="E143" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -3173,9 +2742,6 @@
       <c r="D144" t="n">
         <v>0.7</v>
       </c>
-      <c r="E144" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -3192,9 +2758,6 @@
       <c r="D145" t="n">
         <v>10.4</v>
       </c>
-      <c r="E145" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -3211,9 +2774,6 @@
       <c r="D146" t="n">
         <v>7.1</v>
       </c>
-      <c r="E146" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -3230,9 +2790,6 @@
       <c r="D147" t="n">
         <v>1</v>
       </c>
-      <c r="E147" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -3249,9 +2806,6 @@
       <c r="D148" t="n">
         <v>36</v>
       </c>
-      <c r="E148" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -3268,9 +2822,6 @@
       <c r="D149" t="n">
         <v>25</v>
       </c>
-      <c r="E149" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -3287,9 +2838,6 @@
       <c r="D150" t="n">
         <v>4</v>
       </c>
-      <c r="E150" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -3306,9 +2854,6 @@
       <c r="D151" t="n">
         <v>43.3</v>
       </c>
-      <c r="E151" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -3325,9 +2870,6 @@
       <c r="D152" t="n">
         <v>14</v>
       </c>
-      <c r="E152" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -3344,9 +2886,6 @@
       <c r="D153" t="n">
         <v>2.6</v>
       </c>
-      <c r="E153" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -3363,9 +2902,6 @@
       <c r="D154" t="n">
         <v>63.3</v>
       </c>
-      <c r="E154" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -3382,9 +2918,6 @@
       <c r="D155" t="n">
         <v>3</v>
       </c>
-      <c r="E155" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -3401,9 +2934,6 @@
       <c r="D156" t="n">
         <v>80</v>
       </c>
-      <c r="E156" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -3420,9 +2950,6 @@
       <c r="D157" t="n">
         <v>4.9</v>
       </c>
-      <c r="E157" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -3439,9 +2966,6 @@
       <c r="D158" t="n">
         <v>3</v>
       </c>
-      <c r="E158" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -3458,9 +2982,6 @@
       <c r="D159" t="n">
         <v>5</v>
       </c>
-      <c r="E159" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -3477,9 +2998,6 @@
       <c r="D160" t="n">
         <v>52.3</v>
       </c>
-      <c r="E160" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -3496,9 +3014,6 @@
       <c r="D161" t="n">
         <v>72</v>
       </c>
-      <c r="E161" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -3515,9 +3030,6 @@
       <c r="D162" t="n">
         <v>50.3</v>
       </c>
-      <c r="E162" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -3534,9 +3046,6 @@
       <c r="D163" t="n">
         <v>102</v>
       </c>
-      <c r="E163" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -3553,9 +3062,6 @@
       <c r="D164" t="n">
         <v>4.8</v>
       </c>
-      <c r="E164" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -3572,9 +3078,6 @@
       <c r="D165" t="n">
         <v>11.6</v>
       </c>
-      <c r="E165" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -3591,9 +3094,6 @@
       <c r="D166" t="n">
         <v>0.9</v>
       </c>
-      <c r="E166" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -3610,9 +3110,6 @@
       <c r="D167" t="n">
         <v>18.8</v>
       </c>
-      <c r="E167" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -3629,9 +3126,6 @@
       <c r="D168" t="n">
         <v>11</v>
       </c>
-      <c r="E168" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -3648,9 +3142,6 @@
       <c r="D169" t="n">
         <v>0.7</v>
       </c>
-      <c r="E169" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -3667,9 +3158,6 @@
       <c r="D170" t="n">
         <v>10.4</v>
       </c>
-      <c r="E170" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -3686,9 +3174,6 @@
       <c r="D171" t="n">
         <v>1.7</v>
       </c>
-      <c r="E171" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -3705,9 +3190,6 @@
       <c r="D172" t="n">
         <v>28</v>
       </c>
-      <c r="E172" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -3724,9 +3206,6 @@
       <c r="D173" t="n">
         <v>1</v>
       </c>
-      <c r="E173" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -3743,9 +3222,6 @@
       <c r="D174" t="n">
         <v>41</v>
       </c>
-      <c r="E174" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -3762,9 +3238,6 @@
       <c r="D175" t="n">
         <v>64.2</v>
       </c>
-      <c r="E175" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -3781,9 +3254,6 @@
       <c r="D176" t="n">
         <v>79</v>
       </c>
-      <c r="E176" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -3800,9 +3270,6 @@
       <c r="D177" t="n">
         <v>5</v>
       </c>
-      <c r="E177" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -3819,9 +3286,6 @@
       <c r="D178" t="n">
         <v>9</v>
       </c>
-      <c r="E178" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -3838,9 +3302,6 @@
       <c r="D179" t="n">
         <v>6</v>
       </c>
-      <c r="E179" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -3857,9 +3318,6 @@
       <c r="D180" t="n">
         <v>30</v>
       </c>
-      <c r="E180" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -3876,9 +3334,6 @@
       <c r="D181" t="n">
         <v>10</v>
       </c>
-      <c r="E181" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -3895,9 +3350,6 @@
       <c r="D182" t="n">
         <v>26</v>
       </c>
-      <c r="E182" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -3914,9 +3366,6 @@
       <c r="D183" t="n">
         <v>152.1</v>
       </c>
-      <c r="E183" t="n">
-        <v>2</v>
-      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -3933,9 +3382,6 @@
       <c r="D184" t="n">
         <v>125.4</v>
       </c>
-      <c r="E184" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -3952,9 +3398,6 @@
       <c r="D185" t="n">
         <v>2.5</v>
       </c>
-      <c r="E185" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -3971,9 +3414,6 @@
       <c r="D186" t="n">
         <v>79.2</v>
       </c>
-      <c r="E186" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -3990,9 +3430,6 @@
       <c r="D187" t="n">
         <v>36.1</v>
       </c>
-      <c r="E187" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -4009,9 +3446,6 @@
       <c r="D188" t="n">
         <v>34</v>
       </c>
-      <c r="E188" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -4028,9 +3462,6 @@
       <c r="D189" t="n">
         <v>7.9</v>
       </c>
-      <c r="E189" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -4047,9 +3478,6 @@
       <c r="D190" t="n">
         <v>1.2</v>
       </c>
-      <c r="E190" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -4066,9 +3494,6 @@
       <c r="D191" t="n">
         <v>1</v>
       </c>
-      <c r="E191" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -4085,9 +3510,6 @@
       <c r="D192" t="n">
         <v>7.4</v>
       </c>
-      <c r="E192" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -4104,9 +3526,6 @@
       <c r="D193" t="n">
         <v>6.2</v>
       </c>
-      <c r="E193" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -4123,9 +3542,6 @@
       <c r="D194" t="n">
         <v>10.2</v>
       </c>
-      <c r="E194" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -4142,9 +3558,6 @@
       <c r="D195" t="n">
         <v>4.6</v>
       </c>
-      <c r="E195" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -4161,9 +3574,6 @@
       <c r="D196" t="n">
         <v>71.5</v>
       </c>
-      <c r="E196" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -4180,9 +3590,6 @@
       <c r="D197" t="n">
         <v>14.4</v>
       </c>
-      <c r="E197" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -4199,9 +3606,6 @@
       <c r="D198" t="n">
         <v>1</v>
       </c>
-      <c r="E198" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -4218,9 +3622,6 @@
       <c r="D199" t="n">
         <v>281</v>
       </c>
-      <c r="E199" t="n">
-        <v>2</v>
-      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -4237,9 +3638,6 @@
       <c r="D200" t="n">
         <v>279</v>
       </c>
-      <c r="E200" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -4256,9 +3654,6 @@
       <c r="D201" t="n">
         <v>77</v>
       </c>
-      <c r="E201" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -4275,9 +3670,6 @@
       <c r="D202" t="n">
         <v>88</v>
       </c>
-      <c r="E202" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -4294,9 +3686,6 @@
       <c r="D203" t="n">
         <v>7</v>
       </c>
-      <c r="E203" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -4313,9 +3702,6 @@
       <c r="D204" t="n">
         <v>50.2</v>
       </c>
-      <c r="E204" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -4332,9 +3718,6 @@
       <c r="D205" t="n">
         <v>28.5</v>
       </c>
-      <c r="E205" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -4351,9 +3734,6 @@
       <c r="D206" t="n">
         <v>12.2</v>
       </c>
-      <c r="E206" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -4370,9 +3750,6 @@
       <c r="D207" t="n">
         <v>22</v>
       </c>
-      <c r="E207" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -4389,9 +3766,6 @@
       <c r="D208" t="n">
         <v>0.5</v>
       </c>
-      <c r="E208" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -4408,9 +3782,6 @@
       <c r="D209" t="n">
         <v>5.8</v>
       </c>
-      <c r="E209" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -4427,9 +3798,6 @@
       <c r="D210" t="n">
         <v>13</v>
       </c>
-      <c r="E210" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -4446,9 +3814,6 @@
       <c r="D211" t="n">
         <v>88.5</v>
       </c>
-      <c r="E211" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
@@ -4465,9 +3830,6 @@
       <c r="D212" t="n">
         <v>6</v>
       </c>
-      <c r="E212" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -4484,9 +3846,6 @@
       <c r="D213" t="n">
         <v>24</v>
       </c>
-      <c r="E213" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -4503,9 +3862,6 @@
       <c r="D214" t="n">
         <v>29.2</v>
       </c>
-      <c r="E214" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
@@ -4522,9 +3878,6 @@
       <c r="D215" t="n">
         <v>37</v>
       </c>
-      <c r="E215" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -4541,9 +3894,6 @@
       <c r="D216" t="n">
         <v>34.3</v>
       </c>
-      <c r="E216" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -4560,9 +3910,6 @@
       <c r="D217" t="n">
         <v>23.1</v>
       </c>
-      <c r="E217" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -4579,9 +3926,6 @@
       <c r="D218" t="n">
         <v>13</v>
       </c>
-      <c r="E218" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -4598,9 +3942,6 @@
       <c r="D219" t="n">
         <v>1.2</v>
       </c>
-      <c r="E219" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
@@ -4617,9 +3958,6 @@
       <c r="D220" t="n">
         <v>0.6</v>
       </c>
-      <c r="E220" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -4636,9 +3974,6 @@
       <c r="D221" t="n">
         <v>4</v>
       </c>
-      <c r="E221" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
@@ -4655,9 +3990,6 @@
       <c r="D222" t="n">
         <v>10.5</v>
       </c>
-      <c r="E222" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
@@ -4674,9 +4006,6 @@
       <c r="D223" t="n">
         <v>11</v>
       </c>
-      <c r="E223" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
@@ -4693,9 +4022,6 @@
       <c r="D224" t="n">
         <v>2.7</v>
       </c>
-      <c r="E224" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
@@ -4712,9 +4038,6 @@
       <c r="D225" t="n">
         <v>22</v>
       </c>
-      <c r="E225" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
@@ -4731,9 +4054,6 @@
       <c r="D226" t="n">
         <v>5.4</v>
       </c>
-      <c r="E226" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
@@ -4750,9 +4070,6 @@
       <c r="D227" t="n">
         <v>2</v>
       </c>
-      <c r="E227" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
@@ -4769,9 +4086,6 @@
       <c r="D228" t="n">
         <v>19</v>
       </c>
-      <c r="E228" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
@@ -4788,9 +4102,6 @@
       <c r="D229" t="n">
         <v>1.4</v>
       </c>
-      <c r="E229" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
@@ -4807,9 +4118,6 @@
       <c r="D230" t="n">
         <v>160</v>
       </c>
-      <c r="E230" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
@@ -4826,9 +4134,6 @@
       <c r="D231" t="n">
         <v>4</v>
       </c>
-      <c r="E231" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
@@ -4845,9 +4150,6 @@
       <c r="D232" t="n">
         <v>41</v>
       </c>
-      <c r="E232" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
@@ -4864,9 +4166,6 @@
       <c r="D233" t="n">
         <v>1.5</v>
       </c>
-      <c r="E233" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
@@ -4883,9 +4182,6 @@
       <c r="D234" t="n">
         <v>7</v>
       </c>
-      <c r="E234" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
@@ -4902,9 +4198,6 @@
       <c r="D235" t="n">
         <v>0.6</v>
       </c>
-      <c r="E235" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -4921,9 +4214,6 @@
       <c r="D236" t="n">
         <v>2</v>
       </c>
-      <c r="E236" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
@@ -4940,9 +4230,6 @@
       <c r="D237" t="n">
         <v>69</v>
       </c>
-      <c r="E237" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
@@ -4959,9 +4246,6 @@
       <c r="D238" t="n">
         <v>46.5</v>
       </c>
-      <c r="E238" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
@@ -4978,9 +4262,6 @@
       <c r="D239" t="n">
         <v>12.3</v>
       </c>
-      <c r="E239" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
@@ -4997,9 +4278,6 @@
       <c r="D240" t="n">
         <v>187.7</v>
       </c>
-      <c r="E240" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
@@ -5016,9 +4294,6 @@
       <c r="D241" t="n">
         <v>0.7</v>
       </c>
-      <c r="E241" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
@@ -5035,9 +4310,6 @@
       <c r="D242" t="n">
         <v>29.6</v>
       </c>
-      <c r="E242" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
@@ -5054,9 +4326,6 @@
       <c r="D243" t="n">
         <v>0.6</v>
       </c>
-      <c r="E243" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
@@ -5073,9 +4342,6 @@
       <c r="D244" t="n">
         <v>2</v>
       </c>
-      <c r="E244" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
@@ -5092,9 +4358,6 @@
       <c r="D245" t="n">
         <v>1.1</v>
       </c>
-      <c r="E245" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
@@ -5111,9 +4374,6 @@
       <c r="D246" t="n">
         <v>2</v>
       </c>
-      <c r="E246" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
@@ -5129,9 +4389,6 @@
       </c>
       <c r="D247" t="n">
         <v>10.3</v>
-      </c>
-      <c r="E247" t="n">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>